<commit_message>
fix awful mem allocation & extruder_ct in pticket
</commit_message>
<xml_diff>
--- a/Examples/matmap.xlsx
+++ b/Examples/matmap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noone\Desktop\Tempy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mnoon\deptest\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D9ECD0-2FB2-436B-9129-5761A4341452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF06C293-29DC-4132-9CC2-A3DC12E771CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="2895" windowWidth="25740" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="2280" windowWidth="25740" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>C:\Users\Noone\Desktop\Tempy\Segmentation_brain.stl</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>C:\Users\Noone\Desktop\Tempy\Segmentation_Face.stl</t>
+  </si>
+  <si>
+    <t>segment path</t>
+  </si>
+  <si>
+    <t>poisson's ratio</t>
+  </si>
+  <si>
+    <t>material density</t>
+  </si>
+  <si>
+    <t>youngs modulus</t>
   </si>
 </sst>
 </file>
@@ -370,17 +382,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>

</xml_diff>